<commit_message>
Result [UPDATE], uni_mul_compare [ADD]
</commit_message>
<xml_diff>
--- a/Data_Result/Test_ARIMA_GA_compare.xlsx
+++ b/Data_Result/Test_ARIMA_GA_compare.xlsx
@@ -846,7 +846,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -857,7 +857,7 @@
   <dimension ref="A1:AU59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -3520,68 +3520,74 @@
         <v>26</v>
       </c>
       <c r="B29" s="3">
-        <v>10.989094</v>
+        <v>11.17</v>
       </c>
       <c r="C29" s="3">
-        <v>12.730655</v>
+        <v>11.07</v>
       </c>
       <c r="D29" s="3">
-        <v>13.889756</v>
+        <v>11.48</v>
       </c>
       <c r="E29" s="3">
-        <v>11.732936</v>
+        <v>12.15</v>
       </c>
       <c r="F29" s="3">
-        <v>11.844614</v>
+        <v>10.43</v>
       </c>
       <c r="G29" s="9">
         <v>13.5913067101898</v>
       </c>
-      <c r="H29" s="8"/>
+      <c r="H29" s="38">
+        <v>10.479200000000001</v>
+      </c>
       <c r="I29" s="6">
         <v>16.128499999999999</v>
       </c>
       <c r="J29" s="2">
-        <v>19.534123999999998</v>
+        <v>20.658999999999999</v>
       </c>
       <c r="K29" s="2">
-        <v>17.607855000000001</v>
+        <v>23.6083</v>
       </c>
       <c r="L29" s="2">
-        <v>19.262501</v>
+        <v>22.056799999999999</v>
       </c>
       <c r="M29" s="2">
-        <v>23.233215999999999</v>
+        <v>21.923500000000001</v>
       </c>
       <c r="N29" s="2">
-        <v>19.550640000000001</v>
+        <v>20.722300000000001</v>
       </c>
       <c r="O29" s="9">
         <v>22.864358606187899</v>
       </c>
-      <c r="P29" s="6"/>
+      <c r="P29" s="6">
+        <v>20.476900000000001</v>
+      </c>
       <c r="Q29" s="31">
         <v>26.139600000000002</v>
       </c>
       <c r="R29" s="5">
-        <v>34.003408</v>
+        <v>34.8508</v>
       </c>
       <c r="S29" s="5">
-        <v>46.302984000000002</v>
+        <v>41.492600000000003</v>
       </c>
       <c r="T29" s="5">
-        <v>44.646197999999998</v>
+        <v>54.096400000000003</v>
       </c>
       <c r="U29" s="5">
-        <v>40.460948000000002</v>
+        <v>39.638399999999997</v>
       </c>
       <c r="V29" s="5">
-        <v>33.251849999999997</v>
+        <v>35.268000000000001</v>
       </c>
       <c r="W29" s="1">
         <v>34.749136860687798</v>
       </c>
-      <c r="X29" s="6"/>
+      <c r="X29" s="6">
+        <v>35.487099999999998</v>
+      </c>
       <c r="Y29" s="32">
         <v>43.166899999999998</v>
       </c>
@@ -3611,68 +3617,74 @@
         <v>27</v>
       </c>
       <c r="B30" s="3">
-        <v>13.046882999999999</v>
+        <v>12.94</v>
       </c>
       <c r="C30" s="3">
-        <v>13.216817000000001</v>
+        <v>12.65</v>
       </c>
       <c r="D30" s="3">
-        <v>13.082503000000001</v>
+        <v>12.96</v>
       </c>
       <c r="E30" s="3">
-        <v>13.46644</v>
+        <v>14.27</v>
       </c>
       <c r="F30" s="3">
-        <v>13.827636999999999</v>
+        <v>14.28</v>
       </c>
       <c r="G30" s="9">
         <v>15.103807466993199</v>
       </c>
-      <c r="H30" s="8"/>
+      <c r="H30" s="38">
+        <v>12.4071</v>
+      </c>
       <c r="I30" s="6">
         <v>17.4709</v>
       </c>
       <c r="J30" s="2">
-        <v>20.894523</v>
+        <v>21.585100000000001</v>
       </c>
       <c r="K30" s="2">
-        <v>22.026128</v>
+        <v>22.599</v>
       </c>
       <c r="L30" s="2">
-        <v>21.641888000000002</v>
+        <v>23.5715</v>
       </c>
       <c r="M30" s="2">
-        <v>22.688768</v>
+        <v>22.168700000000001</v>
       </c>
       <c r="N30" s="2">
-        <v>22.90428</v>
+        <v>21.5777</v>
       </c>
       <c r="O30" s="9">
         <v>24.8745184207989</v>
       </c>
-      <c r="P30" s="6"/>
+      <c r="P30" s="6">
+        <v>20.751899999999999</v>
+      </c>
       <c r="Q30" s="31">
         <v>24.552800000000001</v>
       </c>
       <c r="R30" s="5">
-        <v>38.215758999999998</v>
+        <v>39.033700000000003</v>
       </c>
       <c r="S30" s="5">
-        <v>38.333522000000002</v>
+        <v>40.017499999999998</v>
       </c>
       <c r="T30" s="5">
-        <v>39.222507</v>
+        <v>40.534300000000002</v>
       </c>
       <c r="U30" s="5">
-        <v>39.221133000000002</v>
+        <v>42.848100000000002</v>
       </c>
       <c r="V30" s="5">
-        <v>39.522229000000003</v>
+        <v>40.1511</v>
       </c>
       <c r="W30" s="1">
         <v>41.1543503843221</v>
       </c>
-      <c r="X30" s="6"/>
+      <c r="X30" s="6">
+        <v>38.928800000000003</v>
+      </c>
       <c r="Y30" s="32">
         <v>39.750300000000003</v>
       </c>
@@ -6008,23 +6020,23 @@
       </c>
       <c r="B58" s="4">
         <f t="shared" ref="B58:G58" si="0">AVERAGE(B2:B57)</f>
-        <v>11.578124039215684</v>
+        <v>11.579575470588233</v>
       </c>
       <c r="C58" s="4">
         <f t="shared" si="0"/>
-        <v>12.065759980392153</v>
+        <v>12.022084058823525</v>
       </c>
       <c r="D58" s="4">
         <f t="shared" si="0"/>
-        <v>14.647941235294114</v>
+        <v>14.598289098039213</v>
       </c>
       <c r="E58" s="4">
         <f t="shared" si="0"/>
-        <v>12.038685392156859</v>
+        <v>12.062619196078426</v>
       </c>
       <c r="F58" s="4">
         <f t="shared" si="0"/>
-        <v>11.622632098039213</v>
+        <v>11.603764431372547</v>
       </c>
       <c r="G58" s="10">
         <f t="shared" si="0"/>
@@ -6032,7 +6044,7 @@
       </c>
       <c r="H58" s="10">
         <f>AVERAGE(H2:H57)</f>
-        <v>10.727799068181822</v>
+        <v>10.758901282608699</v>
       </c>
       <c r="I58" s="4">
         <f t="shared" ref="I58:O58" si="1">AVERAGE(I2:I57)</f>
@@ -6040,23 +6052,23 @@
       </c>
       <c r="J58" s="4">
         <f t="shared" si="1"/>
-        <v>20.037273137254903</v>
+        <v>20.072870254901961</v>
       </c>
       <c r="K58" s="4">
         <f t="shared" si="1"/>
-        <v>20.591071196078435</v>
+        <v>20.719959764705887</v>
       </c>
       <c r="L58" s="4">
         <f t="shared" si="1"/>
-        <v>20.356468372549017</v>
+        <v>20.449094078431369</v>
       </c>
       <c r="M58" s="4">
         <f t="shared" si="1"/>
-        <v>20.657171529411766</v>
+        <v>20.621293411764711</v>
       </c>
       <c r="N58" s="10">
         <f t="shared" si="1"/>
-        <v>20.641461823529408</v>
+        <v>20.638424176470586</v>
       </c>
       <c r="O58" s="10">
         <f t="shared" si="1"/>
@@ -6064,7 +6076,7 @@
       </c>
       <c r="P58" s="4">
         <f t="shared" ref="P58:Y58" si="2">AVERAGE(P2:P57)</f>
-        <v>18.936352954545459</v>
+        <v>19.009311521739132</v>
       </c>
       <c r="Q58" s="4">
         <f t="shared" si="2"/>
@@ -6072,23 +6084,23 @@
       </c>
       <c r="R58" s="4">
         <f t="shared" si="2"/>
-        <v>34.079889784313735</v>
+        <v>34.112543372549027</v>
       </c>
       <c r="S58" s="4">
         <f t="shared" si="2"/>
-        <v>33.328890313725481</v>
+        <v>33.267588235294106</v>
       </c>
       <c r="T58" s="4">
         <f t="shared" si="2"/>
-        <v>35.822433627450984</v>
+        <v>36.033453137254902</v>
       </c>
       <c r="U58" s="4">
         <f t="shared" si="2"/>
-        <v>33.870096431372545</v>
+        <v>33.925085039215681</v>
       </c>
       <c r="V58" s="4">
         <f t="shared" si="2"/>
-        <v>33.505154921568625</v>
+        <v>33.557018078431376</v>
       </c>
       <c r="W58" s="4">
         <f t="shared" si="2"/>
@@ -6096,7 +6108,7 @@
       </c>
       <c r="X58" s="4">
         <f t="shared" si="2"/>
-        <v>30.394092977272727</v>
+        <v>30.690347630434786</v>
       </c>
       <c r="Y58" s="4">
         <f t="shared" si="2"/>

</xml_diff>